<commit_message>
upd xl in eclipse
</commit_message>
<xml_diff>
--- a/Hello_Lok_ArtId1/src/main/resources/Input1.xlsx
+++ b/Hello_Lok_ArtId1/src/main/resources/Input1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mloke\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mloke\git\Hello_Lok_ArtId1\Hello_Lok_ArtId1\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3C8A54-16E3-4ED0-9DD9-350E52211474}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87597C8C-1FDC-4AB9-AF76-5DF8B6245731}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>a</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
   </si>
 </sst>
 </file>
@@ -351,10 +354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -383,6 +386,14 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
upd xl and file in eclipse
</commit_message>
<xml_diff>
--- a/Hello_Lok_ArtId1/src/main/resources/Input1.xlsx
+++ b/Hello_Lok_ArtId1/src/main/resources/Input1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mloke\git\Hello_Lok_ArtId1\Hello_Lok_ArtId1\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34244627-841C-4AD1-9896-8EEFD7AB3414}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC81D6C-6C47-4354-AEFC-41002A896515}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>a</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
 </sst>
 </file>
@@ -357,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -405,6 +408,14 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
upd xxl in eclip
</commit_message>
<xml_diff>
--- a/Hello_Lok_ArtId1/src/main/resources/Input1.xlsx
+++ b/Hello_Lok_ArtId1/src/main/resources/Input1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mloke\git\Hello_Lok_ArtId1\Hello_Lok_ArtId1\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC81D6C-6C47-4354-AEFC-41002A896515}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D391CB-B656-43E7-B17E-51E8F9160D50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>a</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
   </si>
 </sst>
 </file>
@@ -360,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -416,6 +419,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>